<commit_message>
added blanco y negro y tabla final por secciones
</commit_message>
<xml_diff>
--- a/res/sueldos-s2.xlsx
+++ b/res/sueldos-s2.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lolo\dev\bolciti-excel-analysis\res\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E87099-A7F6-492F-AA74-A8C3F8F8F869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView/>
+    <workbookView xWindow="1440" yWindow="1860" windowWidth="21600" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" r:id="R98acc51b580345d4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="43">
   <si>
     <t xml:space="preserve">Empleado: </t>
   </si>
@@ -100,7 +109,7 @@
     <t>MARTINEZ ANGEL EDUARDO</t>
   </si>
   <si>
-    <t xml:space="preserve">JORGE  LUIS LEITES</t>
+    <t>JORGE  LUIS LEITES</t>
   </si>
   <si>
     <t>MARIO AGUSTIN ALGAÑARAZ</t>
@@ -109,22 +118,22 @@
     <t>CABRERA ALEX EDUARDO</t>
   </si>
   <si>
-    <t xml:space="preserve">BRIAN   NAHUEL   SOTO</t>
+    <t>BRIAN   NAHUEL   SOTO</t>
   </si>
   <si>
-    <t xml:space="preserve">SERGIO   DAMIAN  ARRIETA</t>
+    <t>SERGIO   DAMIAN  ARRIETA</t>
   </si>
   <si>
-    <t xml:space="preserve">ROSA  BEATRIZ  DI  PAOLO</t>
+    <t>ROSA  BEATRIZ  DI  PAOLO</t>
   </si>
   <si>
-    <t xml:space="preserve">BRIZUELA  HERNAN</t>
+    <t>BRIZUELA  HERNAN</t>
   </si>
   <si>
-    <t xml:space="preserve">LEONARDO   LEDESMA</t>
+    <t>LEONARDO   LEDESMA</t>
   </si>
   <si>
-    <t xml:space="preserve">ENRIQUE  CORDOBA</t>
+    <t>ENRIQUE  CORDOBA</t>
   </si>
   <si>
     <t>CRISTIAN DARIO BAEZ</t>
@@ -136,7 +145,7 @@
     <t>JAVIER EDUARDO PAZ</t>
   </si>
   <si>
-    <t xml:space="preserve">MATIAS LEONARDO  MORENO</t>
+    <t>MATIAS LEONARDO  MORENO</t>
   </si>
   <si>
     <t/>
@@ -145,12 +154,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00;[Red]-#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00;[Red]\-#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -167,8 +176,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF" tint="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -180,7 +195,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00008B" tint="0"/>
+        <fgColor rgb="FF00008B"/>
       </patternFill>
     </fill>
   </fills>
@@ -196,45 +211,362 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" xfId="0"/>
-    <xf numFmtId="0" fontId="2" borderId="1" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0"/>
-    <xf numFmtId="0" fontId="1" borderId="2" xfId="0"/>
-    <xf numFmtId="164" fontId="1" borderId="2" xfId="0"/>
-    <xf numFmtId="165" fontId="1" borderId="2" xfId="0"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R272"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -242,22 +574,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:18">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -313,7 +645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:18">
       <c r="A7" s="4">
         <v>3891</v>
       </c>
@@ -369,7 +701,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:18">
       <c r="A8" s="4">
         <v>3892</v>
       </c>
@@ -425,7 +757,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:18">
       <c r="A9" s="4">
         <v>3893</v>
       </c>
@@ -481,7 +813,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:18">
       <c r="A10" s="4">
         <v>3894</v>
       </c>
@@ -527,7 +859,7 @@
       <c r="O10" s="6">
         <v>0</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="7">
         <v>457000</v>
       </c>
       <c r="Q10" s="6">
@@ -537,7 +869,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:18">
       <c r="A11" s="4">
         <v>3895</v>
       </c>
@@ -593,7 +925,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:18">
       <c r="A12" s="4">
         <v>3896</v>
       </c>
@@ -649,7 +981,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:18">
       <c r="A13" s="4">
         <v>3897</v>
       </c>
@@ -705,7 +1037,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:18">
       <c r="A14" s="4">
         <v>3898</v>
       </c>
@@ -761,7 +1093,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:18">
       <c r="A15" s="4">
         <v>3899</v>
       </c>
@@ -817,7 +1149,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:18">
       <c r="A16" s="4">
         <v>3900</v>
       </c>
@@ -873,7 +1205,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:18">
       <c r="A17" s="4">
         <v>3901</v>
       </c>
@@ -929,7 +1261,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:18">
       <c r="A18" s="4">
         <v>3902</v>
       </c>
@@ -985,7 +1317,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:18">
       <c r="A19" s="4">
         <v>3889</v>
       </c>
@@ -1041,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:18">
       <c r="A20" s="4">
         <v>3904</v>
       </c>
@@ -1097,7 +1429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:18">
       <c r="A21" s="4">
         <v>3890</v>
       </c>
@@ -1153,7 +1485,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:18">
       <c r="A22" s="4">
         <v>3879</v>
       </c>
@@ -1209,7 +1541,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:18">
       <c r="A23" s="4">
         <v>3880</v>
       </c>
@@ -1265,7 +1597,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:18">
       <c r="A24" s="4">
         <v>3881</v>
       </c>
@@ -1321,7 +1653,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:18">
       <c r="A25" s="4">
         <v>3882</v>
       </c>
@@ -1377,7 +1709,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:18">
       <c r="A26" s="4">
         <v>3883</v>
       </c>
@@ -1433,7 +1765,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:18">
       <c r="A27" s="4">
         <v>3884</v>
       </c>
@@ -1489,7 +1821,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:18">
       <c r="A28" s="4">
         <v>3885</v>
       </c>
@@ -1545,7 +1877,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:18">
       <c r="A29" s="4">
         <v>3886</v>
       </c>
@@ -1601,7 +1933,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:18">
       <c r="A30" s="4">
         <v>3887</v>
       </c>
@@ -1657,7 +1989,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:18">
       <c r="A31" s="4">
         <v>3888</v>
       </c>
@@ -1713,7 +2045,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:18">
       <c r="A32" s="4">
         <v>3903</v>
       </c>
@@ -1769,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:18">
       <c r="A33" s="4">
         <v>3878</v>
       </c>
@@ -1825,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:18">
       <c r="A34" s="4">
         <v>3866</v>
       </c>
@@ -1881,7 +2213,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:18">
       <c r="A35" s="4">
         <v>3867</v>
       </c>
@@ -1937,7 +2269,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:18">
       <c r="A36" s="4">
         <v>3868</v>
       </c>
@@ -1993,7 +2325,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:18">
       <c r="A37" s="4">
         <v>3869</v>
       </c>
@@ -2049,7 +2381,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:18">
       <c r="A38" s="4">
         <v>3871</v>
       </c>
@@ -2105,7 +2437,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:18">
       <c r="A39" s="4">
         <v>3872</v>
       </c>
@@ -2161,7 +2493,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:18">
       <c r="A40" s="4">
         <v>3873</v>
       </c>
@@ -2217,7 +2549,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:18">
       <c r="A41" s="4">
         <v>3874</v>
       </c>
@@ -2273,7 +2605,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:18">
       <c r="A42" s="4">
         <v>3875</v>
       </c>
@@ -2329,7 +2661,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:18">
       <c r="A43" s="4">
         <v>3876</v>
       </c>
@@ -2385,7 +2717,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:18">
       <c r="A44" s="4">
         <v>3877</v>
       </c>
@@ -2441,7 +2773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:18">
       <c r="A45" s="4">
         <v>3856</v>
       </c>
@@ -2497,7 +2829,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:18">
       <c r="A46" s="4">
         <v>3857</v>
       </c>
@@ -2553,7 +2885,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:18">
       <c r="A47" s="4">
         <v>3858</v>
       </c>
@@ -2609,7 +2941,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:18">
       <c r="A48" s="4">
         <v>3859</v>
       </c>
@@ -2665,7 +2997,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:18">
       <c r="A49" s="4">
         <v>3860</v>
       </c>
@@ -2721,7 +3053,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:18">
       <c r="A50" s="4">
         <v>3861</v>
       </c>
@@ -2777,7 +3109,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:18">
       <c r="A51" s="4">
         <v>3862</v>
       </c>
@@ -2833,7 +3165,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:18">
       <c r="A52" s="4">
         <v>3863</v>
       </c>
@@ -2889,7 +3221,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:18">
       <c r="A53" s="4">
         <v>3864</v>
       </c>
@@ -2945,7 +3277,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:18">
       <c r="A54" s="4">
         <v>3865</v>
       </c>
@@ -3001,7 +3333,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:18">
       <c r="A55" s="4">
         <v>3844</v>
       </c>
@@ -3057,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:18">
       <c r="A56" s="4">
         <v>3845</v>
       </c>
@@ -3113,7 +3445,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:18">
       <c r="A57" s="4">
         <v>3846</v>
       </c>
@@ -3169,7 +3501,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:18">
       <c r="A58" s="4">
         <v>3847</v>
       </c>
@@ -3225,7 +3557,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:18">
       <c r="A59" s="4">
         <v>3848</v>
       </c>
@@ -3281,7 +3613,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:18">
       <c r="A60" s="4">
         <v>3849</v>
       </c>
@@ -3337,7 +3669,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:18">
       <c r="A61" s="4">
         <v>3850</v>
       </c>
@@ -3393,7 +3725,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:18">
       <c r="A62" s="4">
         <v>3851</v>
       </c>
@@ -3449,7 +3781,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:18">
       <c r="A63" s="4">
         <v>3852</v>
       </c>
@@ -3505,7 +3837,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:18">
       <c r="A64" s="4">
         <v>3853</v>
       </c>
@@ -3561,7 +3893,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:18">
       <c r="A65" s="4">
         <v>3854</v>
       </c>
@@ -3617,7 +3949,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:18">
       <c r="A66" s="4">
         <v>3834</v>
       </c>
@@ -3673,7 +4005,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:18">
       <c r="A67" s="4">
         <v>3835</v>
       </c>
@@ -3729,7 +4061,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:18">
       <c r="A68" s="4">
         <v>3836</v>
       </c>
@@ -3785,7 +4117,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:18">
       <c r="A69" s="4">
         <v>3837</v>
       </c>
@@ -3841,7 +4173,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:18">
       <c r="A70" s="4">
         <v>3838</v>
       </c>
@@ -3897,7 +4229,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:18">
       <c r="A71" s="4">
         <v>3839</v>
       </c>
@@ -3953,7 +4285,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:18">
       <c r="A72" s="4">
         <v>3840</v>
       </c>
@@ -4009,7 +4341,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:18">
       <c r="A73" s="4">
         <v>3841</v>
       </c>
@@ -4065,7 +4397,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:18">
       <c r="A74" s="4">
         <v>3842</v>
       </c>
@@ -4121,7 +4453,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:18">
       <c r="A75" s="4">
         <v>3843</v>
       </c>
@@ -4177,7 +4509,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:18">
       <c r="A76" s="4">
         <v>3823</v>
       </c>
@@ -4233,7 +4565,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:18">
       <c r="A77" s="4">
         <v>3824</v>
       </c>
@@ -4289,7 +4621,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:18">
       <c r="A78" s="4">
         <v>3825</v>
       </c>
@@ -4345,7 +4677,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:18">
       <c r="A79" s="4">
         <v>3826</v>
       </c>
@@ -4401,7 +4733,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:18">
       <c r="A80" s="4">
         <v>3827</v>
       </c>
@@ -4457,7 +4789,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:18">
       <c r="A81" s="4">
         <v>3828</v>
       </c>
@@ -4513,7 +4845,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:18">
       <c r="A82" s="4">
         <v>3829</v>
       </c>
@@ -4569,7 +4901,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:18">
       <c r="A83" s="4">
         <v>3830</v>
       </c>
@@ -4625,7 +4957,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:18">
       <c r="A84" s="4">
         <v>3831</v>
       </c>
@@ -4681,7 +5013,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:18">
       <c r="A85" s="4">
         <v>3855</v>
       </c>
@@ -4737,7 +5069,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:18">
       <c r="A86" s="4">
         <v>3833</v>
       </c>
@@ -4793,7 +5125,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:18">
       <c r="A87" s="4">
         <v>3832</v>
       </c>
@@ -4849,7 +5181,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:18">
       <c r="A88" s="4">
         <v>3811</v>
       </c>
@@ -4905,7 +5237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:18">
       <c r="A89" s="4">
         <v>3812</v>
       </c>
@@ -4961,7 +5293,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:18">
       <c r="A90" s="4">
         <v>3813</v>
       </c>
@@ -5017,7 +5349,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:18">
       <c r="A91" s="4">
         <v>3814</v>
       </c>
@@ -5073,7 +5405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:18">
       <c r="A92" s="4">
         <v>3815</v>
       </c>
@@ -5129,7 +5461,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:18">
       <c r="A93" s="4">
         <v>3816</v>
       </c>
@@ -5185,7 +5517,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:18">
       <c r="A94" s="4">
         <v>3817</v>
       </c>
@@ -5241,7 +5573,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:18">
       <c r="A95" s="4">
         <v>3818</v>
       </c>
@@ -5297,7 +5629,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:18">
       <c r="A96" s="4">
         <v>3819</v>
       </c>
@@ -5353,7 +5685,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:18">
       <c r="A97" s="4">
         <v>3820</v>
       </c>
@@ -5409,7 +5741,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:18">
       <c r="A98" s="4">
         <v>3821</v>
       </c>
@@ -5465,7 +5797,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:18">
       <c r="A99" s="4">
         <v>3822</v>
       </c>
@@ -5521,7 +5853,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:18">
       <c r="A100" s="4">
         <v>3810</v>
       </c>
@@ -5577,7 +5909,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:18">
       <c r="A101" s="4">
         <v>3809</v>
       </c>
@@ -5633,7 +5965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:18">
       <c r="A102" s="4">
         <v>3795</v>
       </c>
@@ -5689,7 +6021,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:18">
       <c r="A103" s="4">
         <v>3796</v>
       </c>
@@ -5745,7 +6077,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:18">
       <c r="A104" s="4">
         <v>3797</v>
       </c>
@@ -5801,7 +6133,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:18">
       <c r="A105" s="4">
         <v>3798</v>
       </c>
@@ -5857,7 +6189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:18">
       <c r="A106" s="4">
         <v>3799</v>
       </c>
@@ -5913,7 +6245,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:18">
       <c r="A107" s="4">
         <v>3800</v>
       </c>
@@ -5969,7 +6301,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:18">
       <c r="A108" s="4">
         <v>3801</v>
       </c>
@@ -6025,7 +6357,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:18">
       <c r="A109" s="4">
         <v>3802</v>
       </c>
@@ -6081,7 +6413,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:18">
       <c r="A110" s="4">
         <v>3803</v>
       </c>
@@ -6137,7 +6469,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:18">
       <c r="A111" s="4">
         <v>3804</v>
       </c>
@@ -6193,7 +6525,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:18">
       <c r="A112" s="4">
         <v>3805</v>
       </c>
@@ -6249,7 +6581,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:18">
       <c r="A113" s="4">
         <v>3806</v>
       </c>
@@ -6305,7 +6637,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:18">
       <c r="A114" s="4">
         <v>3807</v>
       </c>
@@ -6361,7 +6693,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:18">
       <c r="A115" s="4">
         <v>3808</v>
       </c>
@@ -6417,7 +6749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:18">
       <c r="A116" s="4">
         <v>3782</v>
       </c>
@@ -6473,7 +6805,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:18">
       <c r="A117" s="4">
         <v>3783</v>
       </c>
@@ -6529,7 +6861,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:18">
       <c r="A118" s="4">
         <v>3784</v>
       </c>
@@ -6585,7 +6917,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:18">
       <c r="A119" s="4">
         <v>3785</v>
       </c>
@@ -6641,7 +6973,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:18">
       <c r="A120" s="4">
         <v>3786</v>
       </c>
@@ -6697,7 +7029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:18">
       <c r="A121" s="4">
         <v>3787</v>
       </c>
@@ -6753,7 +7085,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:18">
       <c r="A122" s="4">
         <v>3788</v>
       </c>
@@ -6809,7 +7141,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:18">
       <c r="A123" s="4">
         <v>3789</v>
       </c>
@@ -6865,7 +7197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:18">
       <c r="A124" s="4">
         <v>3790</v>
       </c>
@@ -6921,7 +7253,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:18">
       <c r="A125" s="4">
         <v>3791</v>
       </c>
@@ -6977,7 +7309,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:18">
       <c r="A126" s="4">
         <v>3792</v>
       </c>
@@ -7033,7 +7365,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:18">
       <c r="A127" s="4">
         <v>3793</v>
       </c>
@@ -7089,7 +7421,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:18">
       <c r="A128" s="4">
         <v>3794</v>
       </c>
@@ -7145,7 +7477,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:18">
       <c r="A129" s="4">
         <v>3771</v>
       </c>
@@ -7201,7 +7533,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:18">
       <c r="A130" s="4">
         <v>3772</v>
       </c>
@@ -7257,7 +7589,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:18">
       <c r="A131" s="4">
         <v>3773</v>
       </c>
@@ -7313,7 +7645,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:18">
       <c r="A132" s="4">
         <v>3774</v>
       </c>
@@ -7369,7 +7701,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:18">
       <c r="A133" s="4">
         <v>3775</v>
       </c>
@@ -7425,7 +7757,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:18">
       <c r="A134" s="4">
         <v>3776</v>
       </c>
@@ -7481,7 +7813,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:18">
       <c r="A135" s="4">
         <v>3777</v>
       </c>
@@ -7537,7 +7869,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:18">
       <c r="A136" s="4">
         <v>3778</v>
       </c>
@@ -7593,7 +7925,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:18">
       <c r="A137" s="4">
         <v>3779</v>
       </c>
@@ -7649,7 +7981,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:18">
       <c r="A138" s="4">
         <v>3780</v>
       </c>
@@ -7705,7 +8037,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:18">
       <c r="A139" s="4">
         <v>3781</v>
       </c>
@@ -7761,7 +8093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:18">
       <c r="A140" s="4">
         <v>3758</v>
       </c>
@@ -7817,7 +8149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:18">
       <c r="A141" s="4">
         <v>3756</v>
       </c>
@@ -7873,7 +8205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:18">
       <c r="A142" s="4">
         <v>3762</v>
       </c>
@@ -7929,7 +8261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:18">
       <c r="A143" s="4">
         <v>3763</v>
       </c>
@@ -7985,7 +8317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:18">
       <c r="A144" s="4">
         <v>3764</v>
       </c>
@@ -8041,7 +8373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:18">
       <c r="A145" s="4">
         <v>3765</v>
       </c>
@@ -8097,7 +8429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:18">
       <c r="A146" s="4">
         <v>3766</v>
       </c>
@@ -8153,7 +8485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:18">
       <c r="A147" s="4">
         <v>3767</v>
       </c>
@@ -8209,7 +8541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:18">
       <c r="A148" s="4">
         <v>3768</v>
       </c>
@@ -8265,7 +8597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:18">
       <c r="A149" s="4">
         <v>3769</v>
       </c>
@@ -8321,7 +8653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:18">
       <c r="A150" s="4">
         <v>3770</v>
       </c>
@@ -8377,7 +8709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:18">
       <c r="A151" s="4">
         <v>3757</v>
       </c>
@@ -8433,7 +8765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:18">
       <c r="A152" s="4">
         <v>3759</v>
       </c>
@@ -8489,7 +8821,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:18">
       <c r="A153" s="4">
         <v>3760</v>
       </c>
@@ -8545,7 +8877,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:18">
       <c r="A154" s="4">
         <v>3761</v>
       </c>
@@ -8601,7 +8933,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:18">
       <c r="A155" s="4">
         <v>3749</v>
       </c>
@@ -8657,7 +8989,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:18">
       <c r="A156" s="4">
         <v>3750</v>
       </c>
@@ -8713,7 +9045,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:18">
       <c r="A157" s="4">
         <v>3751</v>
       </c>
@@ -8769,7 +9101,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:18">
       <c r="A158" s="4">
         <v>3752</v>
       </c>
@@ -8825,7 +9157,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:18">
       <c r="A159" s="4">
         <v>3753</v>
       </c>
@@ -8881,7 +9213,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:18">
       <c r="A160" s="4">
         <v>3754</v>
       </c>
@@ -8937,7 +9269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:18">
       <c r="A161" s="4">
         <v>3755</v>
       </c>
@@ -8993,7 +9325,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:18">
       <c r="A162" s="4">
         <v>3739</v>
       </c>
@@ -9049,7 +9381,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:18">
       <c r="A163" s="4">
         <v>3740</v>
       </c>
@@ -9105,7 +9437,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:18">
       <c r="A164" s="4">
         <v>3741</v>
       </c>
@@ -9161,7 +9493,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:18">
       <c r="A165" s="4">
         <v>3742</v>
       </c>
@@ -9217,7 +9549,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:18">
       <c r="A166" s="4">
         <v>3743</v>
       </c>
@@ -9273,7 +9605,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:18">
       <c r="A167" s="4">
         <v>3744</v>
       </c>
@@ -9329,7 +9661,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:18">
       <c r="A168" s="4">
         <v>3745</v>
       </c>
@@ -9385,7 +9717,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:18">
       <c r="A169" s="4">
         <v>3746</v>
       </c>
@@ -9441,7 +9773,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:18">
       <c r="A170" s="4">
         <v>3747</v>
       </c>
@@ -9497,7 +9829,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:18">
       <c r="A171" s="4">
         <v>3748</v>
       </c>
@@ -9553,7 +9885,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:18">
       <c r="A172" s="4">
         <v>3728</v>
       </c>
@@ -9609,7 +9941,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:18">
       <c r="A173" s="4">
         <v>3729</v>
       </c>
@@ -9665,7 +9997,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:18">
       <c r="A174" s="4">
         <v>3730</v>
       </c>
@@ -9721,7 +10053,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:18">
       <c r="A175" s="4">
         <v>3731</v>
       </c>
@@ -9777,7 +10109,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:18">
       <c r="A176" s="4">
         <v>3732</v>
       </c>
@@ -9833,7 +10165,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:18">
       <c r="A177" s="4">
         <v>3733</v>
       </c>
@@ -9889,7 +10221,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:18">
       <c r="A178" s="4">
         <v>3734</v>
       </c>
@@ -9945,7 +10277,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:18">
       <c r="A179" s="4">
         <v>3735</v>
       </c>
@@ -10001,7 +10333,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:18">
       <c r="A180" s="4">
         <v>3736</v>
       </c>
@@ -10057,7 +10389,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:18">
       <c r="A181" s="4">
         <v>3737</v>
       </c>
@@ -10113,7 +10445,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:18">
       <c r="A182" s="4">
         <v>3738</v>
       </c>
@@ -10169,7 +10501,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:18">
       <c r="A183" s="4">
         <v>3716</v>
       </c>
@@ -10225,7 +10557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:18">
       <c r="A184" s="4">
         <v>3717</v>
       </c>
@@ -10281,7 +10613,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:18">
       <c r="A185" s="4">
         <v>3718</v>
       </c>
@@ -10337,7 +10669,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:18">
       <c r="A186" s="4">
         <v>3719</v>
       </c>
@@ -10393,7 +10725,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:18">
       <c r="A187" s="4">
         <v>3720</v>
       </c>
@@ -10449,7 +10781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:18">
       <c r="A188" s="4">
         <v>3721</v>
       </c>
@@ -10505,7 +10837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:18">
       <c r="A189" s="4">
         <v>3722</v>
       </c>
@@ -10561,7 +10893,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:18">
       <c r="A190" s="4">
         <v>3723</v>
       </c>
@@ -10617,7 +10949,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:18">
       <c r="A191" s="4">
         <v>3724</v>
       </c>
@@ -10673,7 +11005,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:18">
       <c r="A192" s="4">
         <v>3725</v>
       </c>
@@ -10729,7 +11061,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:18">
       <c r="A193" s="4">
         <v>3726</v>
       </c>
@@ -10785,7 +11117,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:18">
       <c r="A194" s="4">
         <v>3727</v>
       </c>
@@ -10841,7 +11173,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:18">
       <c r="A195" s="4">
         <v>3706</v>
       </c>
@@ -10897,7 +11229,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:18">
       <c r="A196" s="4">
         <v>3707</v>
       </c>
@@ -10953,7 +11285,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:18">
       <c r="A197" s="4">
         <v>3708</v>
       </c>
@@ -11009,7 +11341,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:18">
       <c r="A198" s="4">
         <v>3709</v>
       </c>
@@ -11065,7 +11397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:18">
       <c r="A199" s="4">
         <v>3710</v>
       </c>
@@ -11121,7 +11453,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:18">
       <c r="A200" s="4">
         <v>3711</v>
       </c>
@@ -11177,7 +11509,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:18">
       <c r="A201" s="4">
         <v>3712</v>
       </c>
@@ -11233,7 +11565,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="1:18">
       <c r="A202" s="4">
         <v>3713</v>
       </c>
@@ -11289,7 +11621,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="1:18">
       <c r="A203" s="4">
         <v>3714</v>
       </c>
@@ -11345,7 +11677,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="1:18">
       <c r="A204" s="4">
         <v>3715</v>
       </c>
@@ -11401,7 +11733,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="1:18">
       <c r="A205" s="4">
         <v>3695</v>
       </c>
@@ -11457,7 +11789,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:18">
       <c r="A206" s="4">
         <v>3696</v>
       </c>
@@ -11513,7 +11845,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="1:18">
       <c r="A207" s="4">
         <v>3697</v>
       </c>
@@ -11569,7 +11901,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="1:18">
       <c r="A208" s="4">
         <v>3698</v>
       </c>
@@ -11625,7 +11957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="1:18">
       <c r="A209" s="4">
         <v>3699</v>
       </c>
@@ -11681,7 +12013,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="1:18">
       <c r="A210" s="4">
         <v>3700</v>
       </c>
@@ -11737,7 +12069,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="1:18">
       <c r="A211" s="4">
         <v>3701</v>
       </c>
@@ -11793,7 +12125,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="1:18">
       <c r="A212" s="4">
         <v>3702</v>
       </c>
@@ -11849,7 +12181,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="1:18">
       <c r="A213" s="4">
         <v>3703</v>
       </c>
@@ -11905,7 +12237,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="1:18">
       <c r="A214" s="4">
         <v>3704</v>
       </c>
@@ -11961,7 +12293,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="1:18">
       <c r="A215" s="4">
         <v>3705</v>
       </c>
@@ -12017,7 +12349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" spans="1:18">
       <c r="A216" s="4">
         <v>3684</v>
       </c>
@@ -12073,7 +12405,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" spans="1:18">
       <c r="A217" s="4">
         <v>3685</v>
       </c>
@@ -12129,7 +12461,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" spans="1:18">
       <c r="A218" s="4">
         <v>3686</v>
       </c>
@@ -12185,7 +12517,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" spans="1:18">
       <c r="A219" s="4">
         <v>3688</v>
       </c>
@@ -12241,7 +12573,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" spans="1:18">
       <c r="A220" s="4">
         <v>3689</v>
       </c>
@@ -12297,7 +12629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" spans="1:18">
       <c r="A221" s="4">
         <v>3690</v>
       </c>
@@ -12353,7 +12685,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" spans="1:18">
       <c r="A222" s="4">
         <v>3691</v>
       </c>
@@ -12409,7 +12741,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="1:18">
       <c r="A223" s="4">
         <v>3692</v>
       </c>
@@ -12465,7 +12797,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="224">
+    <row r="224" spans="1:18">
       <c r="A224" s="4">
         <v>3693</v>
       </c>
@@ -12521,7 +12853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" spans="1:18">
       <c r="A225" s="4">
         <v>3694</v>
       </c>
@@ -12577,7 +12909,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="226">
+    <row r="226" spans="1:18">
       <c r="A226" s="4">
         <v>3674</v>
       </c>
@@ -12633,7 +12965,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="227">
+    <row r="227" spans="1:18">
       <c r="A227" s="4">
         <v>3675</v>
       </c>
@@ -12689,7 +13021,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="228">
+    <row r="228" spans="1:18">
       <c r="A228" s="4">
         <v>3676</v>
       </c>
@@ -12745,7 +13077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" spans="1:18">
       <c r="A229" s="4">
         <v>3677</v>
       </c>
@@ -12801,7 +13133,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="230">
+    <row r="230" spans="1:18">
       <c r="A230" s="4">
         <v>3678</v>
       </c>
@@ -12857,7 +13189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231">
+    <row r="231" spans="1:18">
       <c r="A231" s="4">
         <v>3679</v>
       </c>
@@ -12913,7 +13245,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="232">
+    <row r="232" spans="1:18">
       <c r="A232" s="4">
         <v>3680</v>
       </c>
@@ -12969,7 +13301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233">
+    <row r="233" spans="1:18">
       <c r="A233" s="4">
         <v>3681</v>
       </c>
@@ -13025,7 +13357,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="234">
+    <row r="234" spans="1:18">
       <c r="A234" s="4">
         <v>3682</v>
       </c>
@@ -13081,7 +13413,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="235">
+    <row r="235" spans="1:18">
       <c r="A235" s="4">
         <v>3683</v>
       </c>
@@ -13137,7 +13469,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="236">
+    <row r="236" spans="1:18">
       <c r="A236" s="4">
         <v>3667</v>
       </c>
@@ -13193,7 +13525,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="237">
+    <row r="237" spans="1:18">
       <c r="A237" s="4">
         <v>3668</v>
       </c>
@@ -13249,7 +13581,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="238">
+    <row r="238" spans="1:18">
       <c r="A238" s="4">
         <v>3669</v>
       </c>
@@ -13305,7 +13637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="239">
+    <row r="239" spans="1:18">
       <c r="A239" s="4">
         <v>3670</v>
       </c>
@@ -13361,7 +13693,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="240">
+    <row r="240" spans="1:18">
       <c r="A240" s="4">
         <v>3671</v>
       </c>
@@ -13417,7 +13749,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="241">
+    <row r="241" spans="1:18">
       <c r="A241" s="4">
         <v>3672</v>
       </c>
@@ -13473,7 +13805,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="242">
+    <row r="242" spans="1:18">
       <c r="A242" s="4">
         <v>3673</v>
       </c>
@@ -13529,7 +13861,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="243">
+    <row r="243" spans="1:18">
       <c r="A243" s="4">
         <v>3652</v>
       </c>
@@ -13585,7 +13917,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="244">
+    <row r="244" spans="1:18">
       <c r="A244" s="4">
         <v>3653</v>
       </c>
@@ -13641,7 +13973,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="245">
+    <row r="245" spans="1:18">
       <c r="A245" s="4">
         <v>3654</v>
       </c>
@@ -13697,7 +14029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246">
+    <row r="246" spans="1:18">
       <c r="A246" s="4">
         <v>3655</v>
       </c>
@@ -13753,7 +14085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="247">
+    <row r="247" spans="1:18">
       <c r="A247" s="4">
         <v>3656</v>
       </c>
@@ -13809,7 +14141,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="248">
+    <row r="248" spans="1:18">
       <c r="A248" s="4">
         <v>3657</v>
       </c>
@@ -13865,7 +14197,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="249">
+    <row r="249" spans="1:18">
       <c r="A249" s="4">
         <v>3658</v>
       </c>
@@ -13921,7 +14253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250">
+    <row r="250" spans="1:18">
       <c r="A250" s="4">
         <v>3659</v>
       </c>
@@ -13977,7 +14309,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="251">
+    <row r="251" spans="1:18">
       <c r="A251" s="4">
         <v>3660</v>
       </c>
@@ -14033,7 +14365,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="252">
+    <row r="252" spans="1:18">
       <c r="A252" s="4">
         <v>3661</v>
       </c>
@@ -14089,7 +14421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253">
+    <row r="253" spans="1:18">
       <c r="A253" s="4">
         <v>3662</v>
       </c>
@@ -14145,7 +14477,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="254">
+    <row r="254" spans="1:18">
       <c r="A254" s="4">
         <v>3663</v>
       </c>
@@ -14201,7 +14533,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="255">
+    <row r="255" spans="1:18">
       <c r="A255" s="4">
         <v>3664</v>
       </c>
@@ -14257,7 +14589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256">
+    <row r="256" spans="1:18">
       <c r="A256" s="4">
         <v>3665</v>
       </c>
@@ -14313,7 +14645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257">
+    <row r="257" spans="1:18">
       <c r="A257" s="4">
         <v>3666</v>
       </c>
@@ -14369,7 +14701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258">
+    <row r="258" spans="1:18">
       <c r="A258" s="4">
         <v>3638</v>
       </c>
@@ -14425,7 +14757,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="259">
+    <row r="259" spans="1:18">
       <c r="A259" s="4">
         <v>3650</v>
       </c>
@@ -14481,7 +14813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260">
+    <row r="260" spans="1:18">
       <c r="A260" s="4">
         <v>3639</v>
       </c>
@@ -14537,7 +14869,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="261">
+    <row r="261" spans="1:18">
       <c r="A261" s="4">
         <v>3640</v>
       </c>
@@ -14593,7 +14925,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="262">
+    <row r="262" spans="1:18">
       <c r="A262" s="4">
         <v>3641</v>
       </c>
@@ -14649,7 +14981,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="263">
+    <row r="263" spans="1:18">
       <c r="A263" s="4">
         <v>3642</v>
       </c>
@@ -14705,7 +15037,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="264">
+    <row r="264" spans="1:18">
       <c r="A264" s="4">
         <v>3643</v>
       </c>
@@ -14761,7 +15093,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="265">
+    <row r="265" spans="1:18">
       <c r="A265" s="4">
         <v>3644</v>
       </c>
@@ -14817,7 +15149,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="266">
+    <row r="266" spans="1:18">
       <c r="A266" s="4">
         <v>3645</v>
       </c>
@@ -14873,7 +15205,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="267">
+    <row r="267" spans="1:18">
       <c r="A267" s="4">
         <v>3646</v>
       </c>
@@ -14929,7 +15261,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="268">
+    <row r="268" spans="1:18">
       <c r="A268" s="4">
         <v>3647</v>
       </c>
@@ -14985,7 +15317,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="269">
+    <row r="269" spans="1:18">
       <c r="A269" s="4">
         <v>3648</v>
       </c>
@@ -15041,7 +15373,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="270">
+    <row r="270" spans="1:18">
       <c r="A270" s="4">
         <v>3649</v>
       </c>
@@ -15097,7 +15429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271">
+    <row r="271" spans="1:18">
       <c r="A271" s="4">
         <v>3620</v>
       </c>
@@ -15153,7 +15485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272">
+    <row r="272" spans="1:18">
       <c r="A272" s="4" t="s">
         <v>42</v>
       </c>
@@ -15210,6 +15542,6 @@
       </c>
     </row>
   </sheetData>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>